<commit_message>
Replace unavailable frag compound. Separate notebooks for frag and drug selection.
</commit_message>
<xml_diff>
--- a/compound_selection/zinc15_eMolecules_intersection_set/20170811_zinc15_eMolecules_subset_group_by_vendor/df_frag_final_supplier_oe.xlsx
+++ b/compound_selection/zinc15_eMolecules_intersection_set/20170811_zinc15_eMolecules_subset_group_by_vendor/df_frag_final_supplier_oe.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="264">
   <si>
     <t>df_frag_final_supplier_oe.csv</t>
   </si>
@@ -82,7 +82,7 @@
     <t>0.7199999690055847</t>
   </si>
   <si>
-    <t>217.22099999999998</t>
+    <t>217.221</t>
   </si>
   <si>
     <t>184.0</t>
@@ -163,6 +163,231 @@
     <t>1327907</t>
   </si>
   <si>
+    <t>Clc1ccc(o1)C(=O)Nc1ccccc1N1CCCCC1</t>
+  </si>
+  <si>
+    <t>[5.346]</t>
+  </si>
+  <si>
+    <t>3.794999837875366</t>
+  </si>
+  <si>
+    <t>304.771</t>
+  </si>
+  <si>
+    <t>424.3</t>
+  </si>
+  <si>
+    <t>148.0</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Enamine Screening Compounds</t>
+  </si>
+  <si>
+    <t>Z119335440</t>
+  </si>
+  <si>
+    <t>c1ccc(c(c1)NC(=O)c2ccc(o2)Cl)N3CCCCC3</t>
+  </si>
+  <si>
+    <t>18908671</t>
+  </si>
+  <si>
+    <t>Clc1ccc(cc1)CNc1ncnc2c1cccc2</t>
+  </si>
+  <si>
+    <t>[5.564]</t>
+  </si>
+  <si>
+    <t>3.523000240325928</t>
+  </si>
+  <si>
+    <t>269.72900000000004</t>
+  </si>
+  <si>
+    <t>415.5</t>
+  </si>
+  <si>
+    <t>Z126957826</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)c(ncn2)NCc3ccc(cc3)Cl</t>
+  </si>
+  <si>
+    <t>30719859</t>
+  </si>
+  <si>
+    <t>O=C(c1cccs1)Nc1nnc(s1)Cc1ccccc1</t>
+  </si>
+  <si>
+    <t>[7.12]</t>
+  </si>
+  <si>
+    <t>3.6050002574920654</t>
+  </si>
+  <si>
+    <t>301.387</t>
+  </si>
+  <si>
+    <t>379.0</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Z27474679</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)Cc2nnc(s2)NC(=O)c3cccs3</t>
+  </si>
+  <si>
+    <t>1228629</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)CNc1ncnc2c1cccc2</t>
+  </si>
+  <si>
+    <t>2.9070003032684326</t>
+  </si>
+  <si>
+    <t>235.284</t>
+  </si>
+  <si>
+    <t>208.7</t>
+  </si>
+  <si>
+    <t>223.0</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Z57161635</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)CNc2c3ccccc3ncn2</t>
+  </si>
+  <si>
+    <t>1327878</t>
+  </si>
+  <si>
+    <t>Brc1cncc(c1)C(=O)Nc1cccc2c1nccc2</t>
+  </si>
+  <si>
+    <t>[4.001, 10.328]</t>
+  </si>
+  <si>
+    <t>2.922999620437622</t>
+  </si>
+  <si>
+    <t>328.163</t>
+  </si>
+  <si>
+    <t>406.0</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>Z28487401</t>
+  </si>
+  <si>
+    <t>c1cc2cccnc2c(c1)NC(=O)c3cc(cnc3)Br</t>
+  </si>
+  <si>
+    <t>18893169</t>
+  </si>
+  <si>
+    <t>OC(=O)Cc1c(=O)[nH]c2c(c1c1ccccc1)cc(cc2)C</t>
+  </si>
+  <si>
+    <t>[4.109]</t>
+  </si>
+  <si>
+    <t>2.8030002117156982</t>
+  </si>
+  <si>
+    <t>293.317</t>
+  </si>
+  <si>
+    <t>232.1</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>Z57157353</t>
+  </si>
+  <si>
+    <t>Cc1ccc2c(c1)c(c(c(=O)[nH]2)CC(=O)O)c3ccccc3</t>
+  </si>
+  <si>
+    <t>1367649</t>
+  </si>
+  <si>
+    <t>COc1cccc(c1)Nc1ncnc2c1cccc2.Cl</t>
+  </si>
+  <si>
+    <t>3.138999938964844</t>
+  </si>
+  <si>
+    <t>287.744</t>
+  </si>
+  <si>
+    <t>119.7</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Z220564816</t>
+  </si>
+  <si>
+    <t>COc1cccc(c1)Nc2c3ccccc3ncn2.Cl</t>
+  </si>
+  <si>
+    <t>1865544</t>
+  </si>
+  <si>
+    <t>Nc1ccc2c(c1)ncn2c1ccccc1</t>
+  </si>
+  <si>
+    <t>[6.348]</t>
+  </si>
+  <si>
+    <t>2.3329999446868896</t>
+  </si>
+  <si>
+    <t>209.247</t>
+  </si>
+  <si>
+    <t>50213.0</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Z57290870</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)n2cnc3c2ccc(c3)N</t>
+  </si>
+  <si>
+    <t>31653344</t>
+  </si>
+  <si>
     <t>Oc1ccc(cc1)n1cnc2c1cccc2</t>
   </si>
   <si>
@@ -178,18 +403,9 @@
     <t>21650.2</t>
   </si>
   <si>
-    <t>148.0</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
-    <t>Enamine Screening Compounds</t>
-  </si>
-  <si>
     <t>Z1318268952</t>
   </si>
   <si>
@@ -199,427 +415,349 @@
     <t>37095168</t>
   </si>
   <si>
-    <t>Nc1ccc2c(c1)ncn2c1ccccc1</t>
-  </si>
-  <si>
-    <t>[6.348]</t>
-  </si>
-  <si>
-    <t>2.3329999446868896</t>
-  </si>
-  <si>
-    <t>209.247</t>
-  </si>
-  <si>
-    <t>50213.0</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Z57290870</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)n2cnc3c2ccc(c3)N</t>
-  </si>
-  <si>
-    <t>31653344</t>
-  </si>
-  <si>
-    <t>O=C(c1n[nH]c2c1cccc2)Nc1ccccc1</t>
-  </si>
-  <si>
-    <t>[8.398]</t>
-  </si>
-  <si>
-    <t>2.6429998874664307</t>
+    <t>O=C(Nc1nc2c(s1)cccc2)CNC(=O)c1ccccc1</t>
+  </si>
+  <si>
+    <t>[8.672]</t>
+  </si>
+  <si>
+    <t>2.7179999351501465</t>
+  </si>
+  <si>
+    <t>311.358</t>
+  </si>
+  <si>
+    <t>149.1</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>Z69130143</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)C(=O)NCC(=O)Nc2nc3ccccc3s2</t>
+  </si>
+  <si>
+    <t>23354217</t>
+  </si>
+  <si>
+    <t>O=C1Nc2c(/C/1=C/c1ccc(cc1)C(C)C)cccc2</t>
+  </si>
+  <si>
+    <t>[3.158]</t>
+  </si>
+  <si>
+    <t>4.2330002784728995</t>
+  </si>
+  <si>
+    <t>263.334</t>
+  </si>
+  <si>
+    <t>283.7</t>
+  </si>
+  <si>
+    <t>400.0</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Life Chemicals</t>
+  </si>
+  <si>
+    <t>F0807-0563</t>
+  </si>
+  <si>
+    <t>CC(C)c1ccc(cc1)/C=C\2/c3ccccc3NC2=O</t>
+  </si>
+  <si>
+    <t>45809595</t>
+  </si>
+  <si>
+    <t>COc1cc2c(ncnc2cc1OC)Nc1cccc(c1)C</t>
+  </si>
+  <si>
+    <t>[4.267]</t>
+  </si>
+  <si>
+    <t>2.5950002670288086</t>
+  </si>
+  <si>
+    <t>295.336</t>
+  </si>
+  <si>
+    <t>1864.0</t>
+  </si>
+  <si>
+    <t>414.0</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Maybridge</t>
+  </si>
+  <si>
+    <t>GK03474</t>
+  </si>
+  <si>
+    <t>Cc1cccc(c1)Nc2c3cc(c(cc3ncn2)OC)OC</t>
+  </si>
+  <si>
+    <t>5828805</t>
+  </si>
+  <si>
+    <t>FC(c1ccc(cc1)c1nnc2n1nc(cc2)NC1CC1)(F)F</t>
+  </si>
+  <si>
+    <t>[4.394]</t>
+  </si>
+  <si>
+    <t>4.128999710083009</t>
+  </si>
+  <si>
+    <t>319.284</t>
+  </si>
+  <si>
+    <t>3175.0</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>RH00113</t>
+  </si>
+  <si>
+    <t>c1cc(ccc1c2nnc3n2nc(cc3)NC4CC4)C(F)(F)F</t>
+  </si>
+  <si>
+    <t>5784088</t>
+  </si>
+  <si>
+    <t>Nc1ncnc2c1cnn2c1ccccc1</t>
+  </si>
+  <si>
+    <t>[3.869]</t>
+  </si>
+  <si>
+    <t>1.4990001916885376</t>
+  </si>
+  <si>
+    <t>211.223</t>
+  </si>
+  <si>
+    <t>3430.0</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>RJC00689</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)n2c3c(cn2)c(ncn3)N</t>
+  </si>
+  <si>
+    <t>719540</t>
+  </si>
+  <si>
+    <t>Clc1cccc(c1)Nc1ncnc2c1cccc2.Cl</t>
+  </si>
+  <si>
+    <t>3.89900016784668</t>
+  </si>
+  <si>
+    <t>292.163</t>
+  </si>
+  <si>
+    <t>7366.0</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>DP00818</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)c(ncn2)Nc3cccc(c3)Cl.Cl</t>
+  </si>
+  <si>
+    <t>1859493</t>
+  </si>
+  <si>
+    <t>Nc1nonc1c1nc2c(n1CC1CC1)cccc2</t>
+  </si>
+  <si>
+    <t>[4.082]</t>
+  </si>
+  <si>
+    <t>2.43999981880188</t>
+  </si>
+  <si>
+    <t>255.275</t>
+  </si>
+  <si>
+    <t>300.0</t>
+  </si>
+  <si>
+    <t>168.0</t>
+  </si>
+  <si>
+    <t>Vitas M Labs</t>
+  </si>
+  <si>
+    <t>STL482461</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)nc(n2CC3CC3)c4c(non4)N</t>
+  </si>
+  <si>
+    <t>8332960</t>
+  </si>
+  <si>
+    <t>O=C(c1c(Cl)cccc1Cl)Nc1ccncc1</t>
+  </si>
+  <si>
+    <t>[4.714, 9.847]</t>
+  </si>
+  <si>
+    <t>2.9270000457763667</t>
+  </si>
+  <si>
+    <t>267.111</t>
+  </si>
+  <si>
+    <t>385.0</t>
+  </si>
+  <si>
+    <t>275.0</t>
+  </si>
+  <si>
+    <t>STK098832</t>
+  </si>
+  <si>
+    <t>c1cc(c(c(c1)Cl)C(=O)Nc2ccncc2)Cl</t>
+  </si>
+  <si>
+    <t>1284691</t>
+  </si>
+  <si>
+    <t>OCCNc1ncnc2c1c(c1ccccc1)c(o2)c1ccccc1</t>
+  </si>
+  <si>
+    <t>[4.294]</t>
+  </si>
+  <si>
+    <t>3.0820000171661377</t>
+  </si>
+  <si>
+    <t>331.36800000000005</t>
+  </si>
+  <si>
+    <t>159.0</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>STK012643</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)c2c3c(ncnc3oc2c4ccccc4)NCCO</t>
+  </si>
+  <si>
+    <t>1415762</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)CSc1nnc(o1)c1ccncc1</t>
+  </si>
+  <si>
+    <t>[4.902]</t>
+  </si>
+  <si>
+    <t>3.3059999942779537</t>
+  </si>
+  <si>
+    <t>269.322</t>
+  </si>
+  <si>
+    <t>170.0</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>STK032731</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)CSc2nnc(o2)c3ccncc3</t>
+  </si>
+  <si>
+    <t>1444229</t>
+  </si>
+  <si>
+    <t>NC(=O)c1ccc2c(c1)nc([nH]2)c1ccccc1</t>
+  </si>
+  <si>
+    <t>[6.342]</t>
+  </si>
+  <si>
+    <t>2.1920003890991206</t>
   </si>
   <si>
     <t>237.257</t>
   </si>
   <si>
-    <t>762.8</t>
-  </si>
-  <si>
-    <t>223.0</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>Z31504656</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)NC(=O)c2c3ccccc3[nH]n2</t>
-  </si>
-  <si>
-    <t>13419113</t>
-  </si>
-  <si>
-    <t>COc1cccc(c1)Nc1ncnc2c1cccc2.Cl</t>
-  </si>
-  <si>
-    <t>3.1389999389648438</t>
-  </si>
-  <si>
-    <t>287.744</t>
-  </si>
-  <si>
-    <t>119.7</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>Z220564816</t>
-  </si>
-  <si>
-    <t>COc1cccc(c1)Nc2c3ccccc3ncn2.Cl</t>
-  </si>
-  <si>
-    <t>1865544</t>
-  </si>
-  <si>
-    <t>OC(=O)Cc1c(=O)[nH]c2c(c1c1ccccc1)cc(cc2)C</t>
-  </si>
-  <si>
-    <t>[4.109]</t>
-  </si>
-  <si>
-    <t>2.8030002117156982</t>
-  </si>
-  <si>
-    <t>293.317</t>
-  </si>
-  <si>
-    <t>232.1</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Z57157353</t>
-  </si>
-  <si>
-    <t>Cc1ccc2c(c1)c(c(c(=O)[nH]2)CC(=O)O)c3ccccc3</t>
-  </si>
-  <si>
-    <t>1367649</t>
-  </si>
-  <si>
-    <t>O=C(Nc1nc2c(s1)cccc2)CNC(=O)c1ccccc1</t>
-  </si>
-  <si>
-    <t>[8.672]</t>
-  </si>
-  <si>
-    <t>2.7179999351501465</t>
-  </si>
-  <si>
-    <t>311.358</t>
-  </si>
-  <si>
-    <t>149.1</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>Z69130143</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)C(=O)NCC(=O)Nc2nc3ccccc3s2</t>
-  </si>
-  <si>
-    <t>23354217</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)CNc1ncnc2c1cccc2</t>
-  </si>
-  <si>
-    <t>[5.564]</t>
-  </si>
-  <si>
-    <t>2.9070003032684326</t>
-  </si>
-  <si>
-    <t>235.28400000000002</t>
-  </si>
-  <si>
-    <t>208.7</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Z57161635</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)CNc2c3ccccc3ncn2</t>
-  </si>
-  <si>
-    <t>1327878</t>
-  </si>
-  <si>
-    <t>O=C(c1cccs1)Nc1nnc(s1)Cc1ccccc1</t>
-  </si>
-  <si>
-    <t>[7.12]</t>
-  </si>
-  <si>
-    <t>3.6050002574920654</t>
-  </si>
-  <si>
-    <t>301.387</t>
-  </si>
-  <si>
-    <t>379.0</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>Z27474679</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)Cc2nnc(s2)NC(=O)c3cccs3</t>
-  </si>
-  <si>
-    <t>1228629</t>
-  </si>
-  <si>
-    <t>Clc1ccc(cc1)CNc1ncnc2c1cccc2</t>
-  </si>
-  <si>
-    <t>3.523000240325928</t>
-  </si>
-  <si>
-    <t>269.72900000000004</t>
-  </si>
-  <si>
-    <t>415.5</t>
-  </si>
-  <si>
-    <t>Z126957826</t>
-  </si>
-  <si>
-    <t>c1ccc2c(c1)c(ncn2)NCc3ccc(cc3)Cl</t>
-  </si>
-  <si>
-    <t>30719859</t>
-  </si>
-  <si>
-    <t>Clc1ccc(o1)C(=O)Nc1ccccc1N1CCCCC1</t>
-  </si>
-  <si>
-    <t>[5.346]</t>
-  </si>
-  <si>
-    <t>3.794999837875366</t>
-  </si>
-  <si>
-    <t>304.77099999999996</t>
-  </si>
-  <si>
-    <t>424.3</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>Z119335440</t>
-  </si>
-  <si>
-    <t>c1ccc(c(c1)NC(=O)c2ccc(o2)Cl)N3CCCCC3</t>
-  </si>
-  <si>
-    <t>18908671</t>
-  </si>
-  <si>
-    <t>Brc1cncc(c1)C(=O)Nc1cccc2c1nccc2</t>
-  </si>
-  <si>
-    <t>[4.001, 10.328]</t>
-  </si>
-  <si>
-    <t>2.922999620437622</t>
-  </si>
-  <si>
-    <t>328.163</t>
-  </si>
-  <si>
-    <t>406.0</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>Z28487401</t>
-  </si>
-  <si>
-    <t>c1cc2cccnc2c(c1)NC(=O)c3cc(cnc3)Br</t>
-  </si>
-  <si>
-    <t>18893169</t>
-  </si>
-  <si>
-    <t>O=C1Nc2c(/C/1=C/c1ccc(cc1)C(C)C)cccc2</t>
-  </si>
-  <si>
-    <t>[3.158]</t>
-  </si>
-  <si>
-    <t>4.2330002784729</t>
-  </si>
-  <si>
-    <t>263.334</t>
-  </si>
-  <si>
-    <t>283.7</t>
-  </si>
-  <si>
-    <t>400.0</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Life Chemicals</t>
-  </si>
-  <si>
-    <t>F0807-0563</t>
-  </si>
-  <si>
-    <t>CC(C)c1ccc(cc1)/C=C\2/c3ccccc3NC2=O</t>
-  </si>
-  <si>
-    <t>45809595</t>
-  </si>
-  <si>
-    <t>Clc1cccc(c1)Nc1ncnc2c1cccc2.Cl</t>
-  </si>
-  <si>
-    <t>3.89900016784668</t>
-  </si>
-  <si>
-    <t>292.163</t>
-  </si>
-  <si>
-    <t>7366.0</t>
-  </si>
-  <si>
-    <t>414.0</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Maybridge</t>
-  </si>
-  <si>
-    <t>DP00818</t>
-  </si>
-  <si>
-    <t>c1ccc2c(c1)c(ncn2)Nc3cccc(c3)Cl.Cl</t>
-  </si>
-  <si>
-    <t>1859493</t>
-  </si>
-  <si>
-    <t>Nc1ncnc2c1cnn2c1ccccc1</t>
-  </si>
-  <si>
-    <t>[3.869]</t>
-  </si>
-  <si>
-    <t>1.4990001916885376</t>
-  </si>
-  <si>
-    <t>211.22299999999998</t>
-  </si>
-  <si>
-    <t>3430.0</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>RJC00689</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)n2c3c(cn2)c(ncn3)N</t>
-  </si>
-  <si>
-    <t>719540</t>
-  </si>
-  <si>
-    <t>COc1cc2c(ncnc2cc1OC)Nc1cccc(c1)C</t>
-  </si>
-  <si>
-    <t>[4.267]</t>
-  </si>
-  <si>
-    <t>2.5950002670288086</t>
-  </si>
-  <si>
-    <t>295.336</t>
-  </si>
-  <si>
-    <t>1864.0</t>
-  </si>
-  <si>
-    <t>GK03474</t>
-  </si>
-  <si>
-    <t>Cc1cccc(c1)Nc2c3cc(c(cc3ncn2)OC)OC</t>
-  </si>
-  <si>
-    <t>5828805</t>
-  </si>
-  <si>
-    <t>FC(c1ccc(cc1)c1nnc2n1nc(cc2)NC1CC1)(F)F</t>
-  </si>
-  <si>
-    <t>[4.394]</t>
-  </si>
-  <si>
-    <t>4.128999710083009</t>
-  </si>
-  <si>
-    <t>319.284</t>
-  </si>
-  <si>
-    <t>3175.0</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>RH00113</t>
-  </si>
-  <si>
-    <t>c1cc(ccc1c2nnc3n2nc(cc3)NC4CC4)C(F)(F)F</t>
-  </si>
-  <si>
-    <t>5784088</t>
+    <t>2000.0</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>STL497402</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)c2[nH]c3ccc(cc3n2)C(=O)N</t>
+  </si>
+  <si>
+    <t>37053191</t>
+  </si>
+  <si>
+    <t>Cc1ccc(cc1)S(=O)(=O)Nc1cccc(c1)C(F)(F)F</t>
+  </si>
+  <si>
+    <t>[7.903]</t>
+  </si>
+  <si>
+    <t>3.747999668121338</t>
+  </si>
+  <si>
+    <t>315.311</t>
+  </si>
+  <si>
+    <t>527.0</t>
+  </si>
+  <si>
+    <t>STK053880</t>
+  </si>
+  <si>
+    <t>Cc1ccc(cc1)S(=O)(=O)Nc2cccc(c2)C(F)(F)F</t>
+  </si>
+  <si>
+    <t>1377874</t>
   </si>
   <si>
     <t>O=C1S/C(=C/c2ccc(o2)c2ccc(c(c2)Cl)F)/C(=O)N1</t>
@@ -637,12 +775,6 @@
     <t>125.0</t>
   </si>
   <si>
-    <t>168.0</t>
-  </si>
-  <si>
-    <t>Vitas M Labs</t>
-  </si>
-  <si>
     <t>STL282834</t>
   </si>
   <si>
@@ -652,132 +784,6 @@
     <t>25775231</t>
   </si>
   <si>
-    <t>Nc1nonc1c1nc2c(n1CC1CC1)cccc2</t>
-  </si>
-  <si>
-    <t>[4.082]</t>
-  </si>
-  <si>
-    <t>2.43999981880188</t>
-  </si>
-  <si>
-    <t>255.275</t>
-  </si>
-  <si>
-    <t>300.0</t>
-  </si>
-  <si>
-    <t>STL482461</t>
-  </si>
-  <si>
-    <t>c1ccc2c(c1)nc(n2CC3CC3)c4c(non4)N</t>
-  </si>
-  <si>
-    <t>8332960</t>
-  </si>
-  <si>
-    <t>OCCNc1ncnc2c1c(c1ccccc1)c(o2)c1ccccc1</t>
-  </si>
-  <si>
-    <t>[4.294]</t>
-  </si>
-  <si>
-    <t>3.0820000171661377</t>
-  </si>
-  <si>
-    <t>331.36800000000005</t>
-  </si>
-  <si>
-    <t>159.0</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>STK012643</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)c2c3c(ncnc3oc2c4ccccc4)NCCO</t>
-  </si>
-  <si>
-    <t>1415762</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)CSc1nnc(o1)c1ccncc1</t>
-  </si>
-  <si>
-    <t>[4.902]</t>
-  </si>
-  <si>
-    <t>3.3059999942779537</t>
-  </si>
-  <si>
-    <t>269.322</t>
-  </si>
-  <si>
-    <t>170.0</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>STK032731</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)CSc2nnc(o2)c3ccncc3</t>
-  </si>
-  <si>
-    <t>1444229</t>
-  </si>
-  <si>
-    <t>NC(=O)c1ccc2c(c1)nc([nH]2)c1ccccc1</t>
-  </si>
-  <si>
-    <t>[6.342]</t>
-  </si>
-  <si>
-    <t>2.1920003890991206</t>
-  </si>
-  <si>
-    <t>2000.0</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>STL497402</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)c2[nH]c3ccc(cc3n2)C(=O)N</t>
-  </si>
-  <si>
-    <t>37053191</t>
-  </si>
-  <si>
-    <t>Cc1ccc(cc1)S(=O)(=O)Nc1cccc(c1)C(F)(F)F</t>
-  </si>
-  <si>
-    <t>[7.903]</t>
-  </si>
-  <si>
-    <t>3.747999668121338</t>
-  </si>
-  <si>
-    <t>315.311</t>
-  </si>
-  <si>
-    <t>527.0</t>
-  </si>
-  <si>
-    <t>STK053880</t>
-  </si>
-  <si>
-    <t>Cc1ccc(cc1)S(=O)(=O)Nc2cccc(c2)C(F)(F)F</t>
-  </si>
-  <si>
-    <t>1377874</t>
-  </si>
-  <si>
     <t>COc1cc(ccc1OC)c1csc(c1C(=O)OC(C)C)N</t>
   </si>
   <si>
@@ -787,7 +793,7 @@
     <t>4.079999923706056</t>
   </si>
   <si>
-    <t>321.39099999999996</t>
+    <t>321.391</t>
   </si>
   <si>
     <t>10117.0</t>
@@ -2359,7 +2365,7 @@
         <v>25</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>55</v>
@@ -2412,19 +2418,19 @@
         <v>25</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>31</v>
@@ -2433,48 +2439,48 @@
         <v>57</v>
       </c>
       <c r="P6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q6" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="R6" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>28</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>30</v>
@@ -2486,33 +2492,33 @@
         <v>57</v>
       </c>
       <c r="P7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:18" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>25</v>
@@ -2530,7 +2536,7 @@
         <v>84</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="N8" s="3" t="s">
         <v>31</v>
@@ -2565,7 +2571,7 @@
         <v>92</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>25</v>
@@ -2580,10 +2586,10 @@
         <v>28</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>31</v>
@@ -2592,51 +2598,51 @@
         <v>57</v>
       </c>
       <c r="P9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q9" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="R9" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:18" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B10" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>103</v>
+        <v>42</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="N10" s="3" t="s">
         <v>31</v>
@@ -2645,33 +2651,33 @@
         <v>57</v>
       </c>
       <c r="P10" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="R10" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:18" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B11" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>25</v>
@@ -2686,10 +2692,10 @@
         <v>28</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>31</v>
@@ -2698,30 +2704,30 @@
         <v>57</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:18" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B12" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>54</v>
@@ -2730,16 +2736,16 @@
         <v>25</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>122</v>
+        <v>30</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>30</v>
@@ -2751,30 +2757,30 @@
         <v>57</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:18" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>54</v>
@@ -2783,19 +2789,19 @@
         <v>25</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>28</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>31</v>
@@ -2804,30 +2810,30 @@
         <v>57</v>
       </c>
       <c r="P13" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q13" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="R13" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:18" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>54</v>
@@ -2836,16 +2842,16 @@
         <v>25</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>139</v>
+        <v>75</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>30</v>
@@ -2883,22 +2889,22 @@
         <v>147</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>113</v>
+        <v>150</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>30</v>
@@ -2907,104 +2913,104 @@
         <v>31</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B16" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>158</v>
+        <v>43</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>31</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="2:18" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B17" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>37</v>
+        <v>167</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>43</v>
+        <v>171</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>28</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>45</v>
@@ -3013,36 +3019,36 @@
         <v>31</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="2:18" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B18" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>25</v>
@@ -3051,13 +3057,13 @@
         <v>30</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="M18" s="3" t="s">
         <v>30</v>
@@ -3066,42 +3072,42 @@
         <v>31</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="2:18" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B19" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>185</v>
+        <v>37</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>43</v>
@@ -3110,7 +3116,7 @@
         <v>28</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>76</v>
+        <v>190</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>45</v>
@@ -3119,51 +3125,51 @@
         <v>31</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="2:18" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B20" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>168</v>
+        <v>199</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>197</v>
+        <v>139</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>198</v>
+        <v>120</v>
       </c>
       <c r="M20" s="3" t="s">
         <v>45</v>
@@ -3172,104 +3178,104 @@
         <v>31</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="2:18" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B21" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>28</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>169</v>
+        <v>84</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>31</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="2:18" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B22" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>104</v>
+        <v>218</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="M22" s="3" t="s">
         <v>45</v>
@@ -3278,151 +3284,151 @@
         <v>31</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="2:18" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B23" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>122</v>
+        <v>29</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>28</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>31</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="2:18" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B24" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>31</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="2:18" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B25" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>73</v>
+        <v>243</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>242</v>
+        <v>149</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>28</v>
@@ -3437,104 +3443,104 @@
         <v>31</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="2:18" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B26" s="3" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>139</v>
+        <v>190</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="N26" s="3" t="s">
         <v>31</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="27" spans="2:18" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B27" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>103</v>
+        <v>138</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>28</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>30</v>
@@ -3543,16 +3549,16 @@
         <v>31</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>